<commit_message>
processes data txt file
</commit_message>
<xml_diff>
--- a/athena/processes_test/processes_data1.xlsx
+++ b/athena/processes_test/processes_data1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\reu2024\research\summer2024\athena\processes_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BB3178-C7C8-47D9-B58C-756CD73F6EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE05648-636B-4D20-9BA6-148C7DEC62F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,6 +160,12 @@
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -179,6 +185,9 @@
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -195,15 +204,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2393,15 +2393,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CFAB3D3-A091-41F6-8EFB-906801341DFF}" name="Table22" displayName="Table22" ref="I2:M35" totalsRowCount="1">
   <autoFilter ref="I2:M34" xr:uid="{0CFAB3D3-A091-41F6-8EFB-906801341DFF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2870F720-140F-4DAE-9CF8-03FD0B6FEB20}" name="Processes" totalsRowLabel="Total Time" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B8121DE1-6D1D-4DDE-A11F-F8DF2BF67D5B}" name="Computation Time (s)" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="1">
+    <tableColumn id="1" xr3:uid="{2870F720-140F-4DAE-9CF8-03FD0B6FEB20}" name="Processes" totalsRowLabel="Total Time" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B8121DE1-6D1D-4DDE-A11F-F8DF2BF67D5B}" name="Computation Time (s)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="3">
       <totalsRowFormula>SUM(Table22[Computation Time (s)])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{81C9C330-7E24-4135-8119-5CFC2CB0F8DA}" name="Computation Time (min)" totalsRowLabel="sec" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{81C9C330-7E24-4135-8119-5CFC2CB0F8DA}" name="Computation Time (min)" totalsRowLabel="sec" dataDxfId="2">
       <calculatedColumnFormula>Table22[[#This Row],[Computation Time (s)]]/60</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AA2F2E7B-7D50-4D56-A974-28DD619A7DB7}" name="Cycles"/>
-    <tableColumn id="5" xr3:uid="{8818B97D-09D4-48A7-B16C-A3E419F56485}" name="Cycles/Second" dataDxfId="3" totalsRowDxfId="0">
+    <tableColumn id="5" xr3:uid="{8818B97D-09D4-48A7-B16C-A3E419F56485}" name="Cycles/Second" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>Table22[[#This Row],[Cycles]]/Table22[[#This Row],[Computation Time (s)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2675,7 +2675,7 @@
   <dimension ref="F1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I2" sqref="I2:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>